<commit_message>
[Modify]S0072 40030 40090 40110
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40030.xlsx
+++ b/PhoenixCI/Excel_Template/40030.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandylo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\PB\CI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7965" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="保證金(Fut)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="107">
   <si>
     <r>
       <rPr>
@@ -842,32 +842,6 @@
   </si>
   <si>
     <r>
-      <t>JPX
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>日幣</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>SGX
 (</t>
     </r>
@@ -1455,6 +1429,10 @@
       <t>保證金占契約價值比與國際主要交易所比較表</t>
     </r>
     <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料日期：2018年12月4日</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4931,7 +4909,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="55"/>
       <c r="D3" s="56"/>
@@ -4941,7 +4919,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>41</v>
@@ -4949,7 +4927,7 @@
     </row>
     <row r="5" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
@@ -4980,14 +4958,14 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="56"/>
@@ -4997,7 +4975,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>41</v>
@@ -5005,7 +4983,7 @@
     </row>
     <row r="12" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="25"/>
@@ -5036,7 +5014,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
@@ -5108,7 +5086,7 @@
     <row r="4" spans="2:8" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>52</v>
@@ -5117,7 +5095,7 @@
         <v>51</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>52</v>
@@ -5177,25 +5155,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H7"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="8" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="6" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="31"/>
-      <c r="H1" s="31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
         <v>65</v>
       </c>
@@ -5203,10 +5180,8 @@
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-    </row>
-    <row r="3" spans="2:8" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:6" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="52" t="s">
         <v>25</v>
       </c>
@@ -5214,73 +5189,59 @@
         <v>48</v>
       </c>
       <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53" t="s">
+      <c r="E3" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-    </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="2:6" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5312,7 +5273,7 @@
     </row>
     <row r="2" spans="2:6" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -5335,21 +5296,21 @@
     <row r="4" spans="2:6" s="4" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -5411,7 +5372,7 @@
     </row>
     <row r="2" spans="2:6" s="29" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -5434,21 +5395,21 @@
     <row r="4" spans="2:6" s="4" customFormat="1" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -5506,12 +5467,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="2:6" s="29" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
@@ -5523,32 +5484,32 @@
         <v>25</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="53"/>
       <c r="E3" s="53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" s="53"/>
     </row>
     <row r="4" spans="2:6" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
       <c r="C4" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>95</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -5557,7 +5518,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
@@ -5566,7 +5527,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
@@ -5608,7 +5569,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -5633,21 +5594,21 @@
       <c r="A4" s="4"/>
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>89</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -5693,7 +5654,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="10"/>
     <col min="2" max="2" width="11.625" style="10" customWidth="1"/>
@@ -7083,8 +7044,6 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
     <mergeCell ref="B21:H21"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B49:H49"/>
@@ -7099,8 +7058,6 @@
     <mergeCell ref="C45:E45"/>
     <mergeCell ref="F45:H45"/>
     <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B28:H28"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="B16:H16"/>
@@ -7113,11 +7070,15 @@
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="B24:B25"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B28:H28"/>
     <mergeCell ref="B58:H58"/>
     <mergeCell ref="B59:B60"/>
     <mergeCell ref="C59:E59"/>
@@ -9233,8 +9194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -9251,7 +9212,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -9276,21 +9237,21 @@
       <c r="A4" s="4"/>
       <c r="B4" s="52"/>
       <c r="C4" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="33" t="s">
-        <v>104</v>
-      </c>
       <c r="F4" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -9641,7 +9602,7 @@
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -9736,7 +9697,7 @@
     </row>
     <row r="15" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -9834,7 +9795,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
@@ -9890,7 +9851,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
@@ -9985,7 +9946,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
@@ -10041,7 +10002,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
@@ -10087,7 +10048,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="55"/>
       <c r="D3" s="56"/>
@@ -10097,7 +10058,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>41</v>
@@ -10105,7 +10066,7 @@
     </row>
     <row r="5" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
@@ -10136,14 +10097,14 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="56"/>
@@ -10153,7 +10114,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>41</v>
@@ -10161,7 +10122,7 @@
     </row>
     <row r="12" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B12" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="25"/>
@@ -10192,7 +10153,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>

</xml_diff>